<commit_message>
bug fixing konfirmasi harga
</commit_message>
<xml_diff>
--- a/documents/Tasklist Baragud.xlsx
+++ b/documents/Tasklist Baragud.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
   <si>
     <t>Lupa Password</t>
   </si>
@@ -643,11 +643,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -955,7 +955,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1543,7 +1543,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18:D19"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,10 +1559,10 @@
       <c r="C2" s="7"/>
     </row>
     <row r="4" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="8" t="s">
         <v>16</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>131</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1628,7 +1628,7 @@
       <c r="C7" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>131</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1650,7 +1650,7 @@
       </c>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>131</v>
       </c>
       <c r="E11" s="2">
@@ -1661,7 +1661,7 @@
       </c>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>131</v>
       </c>
       <c r="E12" s="2">
@@ -1675,7 +1675,7 @@
       </c>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>131</v>
       </c>
       <c r="E13" s="2"/>
@@ -1687,7 +1687,7 @@
       </c>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>131</v>
       </c>
       <c r="E14" s="2"/>
@@ -1699,7 +1699,7 @@
       </c>
     </row>
     <row r="15" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>131</v>
       </c>
       <c r="E15" s="2"/>
@@ -1711,7 +1711,7 @@
       </c>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>131</v>
       </c>
       <c r="E16" s="2"/>
@@ -1726,7 +1726,7 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>131</v>
       </c>
       <c r="E18" s="2">
@@ -1737,7 +1737,7 @@
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>131</v>
       </c>
       <c r="E19" s="2">
@@ -1762,6 +1762,9 @@
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="E23" s="2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
New Structure & Dummy Data Baragud
</commit_message>
<xml_diff>
--- a/documents/Tasklist Baragud.xlsx
+++ b/documents/Tasklist Baragud.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\git\socfin\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85787EC-2BDD-49D5-94C1-1A14215F4978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="2" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="134">
   <si>
     <t>Lupa Password</t>
   </si>
@@ -532,11 +538,17 @@
   <si>
     <t>Done</t>
   </si>
+  <si>
+    <t>23.Jun.2022</t>
+  </si>
+  <si>
+    <t>Perdi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -955,14 +967,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AG116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -970,18 +982,18 @@
       <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" customWidth="1"/>
+    <col min="2" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
@@ -1023,392 +1035,392 @@
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
     </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:33" x14ac:dyDescent="0.3">
       <c r="F4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:33" x14ac:dyDescent="0.3">
       <c r="F5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:33" x14ac:dyDescent="0.3">
       <c r="F6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:33" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:33" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:33" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:33" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:33" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:33" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:33" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G27" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F36" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F38" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H42" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H47" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H48" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F49" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F51" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F53" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F55" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F56" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F57" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F58" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H59" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H60" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F61" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H62" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H63" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H64" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F65" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F66" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F67" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F69" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F70" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F71" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F72" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F73" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F74" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H75" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H76" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="77" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F77" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F78" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="79" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="6:8" x14ac:dyDescent="0.3">
       <c r="H80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F82" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F83" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F84" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F85" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F86" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F87" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F88" t="s">
         <v>110</v>
       </c>
@@ -1416,107 +1428,107 @@
         <v>111</v>
       </c>
     </row>
-    <row r="89" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F89" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F90" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="93" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F93" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="94" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F94" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F95" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F96" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F97" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F98" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F99" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F101" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F103" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F104" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F105" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F106" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F107" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F109" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F111" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F112" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="113" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F113" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="6:11" x14ac:dyDescent="0.3">
       <c r="G114" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="115" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="6:11" x14ac:dyDescent="0.3">
       <c r="H115" t="s">
         <v>114</v>
       </c>
@@ -1524,7 +1536,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="116" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="6:11" x14ac:dyDescent="0.3">
       <c r="J116">
         <v>20.004000000000001</v>
       </c>
@@ -1538,27 +1550,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AE26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:AE32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23:D25"/>
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD17" sqref="AD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="5.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:31" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:31" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="7"/>
     </row>
-    <row r="4" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:31" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>125</v>
       </c>
@@ -1596,7 +1608,7 @@
       <c r="AD4" s="6"/>
       <c r="AE4" s="6"/>
     </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -1607,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -1624,7 +1636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:31" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>127</v>
       </c>
@@ -1638,18 +1650,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:31" x14ac:dyDescent="0.3">
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:31" x14ac:dyDescent="0.3">
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.3">
       <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.3">
       <c r="D11" s="9" t="s">
         <v>131</v>
       </c>
@@ -1660,7 +1672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.3">
       <c r="D12" s="9" t="s">
         <v>131</v>
       </c>
@@ -1674,7 +1686,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.3">
       <c r="D13" s="9" t="s">
         <v>131</v>
       </c>
@@ -1686,7 +1698,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:31" x14ac:dyDescent="0.3">
       <c r="D14" s="9" t="s">
         <v>131</v>
       </c>
@@ -1698,7 +1710,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:31" x14ac:dyDescent="0.3">
       <c r="D15" s="9" t="s">
         <v>131</v>
       </c>
@@ -1710,7 +1722,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.3">
       <c r="D16" s="9" t="s">
         <v>131</v>
       </c>
@@ -1719,13 +1731,13 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E17" s="2"/>
       <c r="G17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D18" s="9" t="s">
         <v>131</v>
       </c>
@@ -1736,7 +1748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D19" s="9" t="s">
         <v>131</v>
       </c>
@@ -1747,21 +1759,21 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E20" s="2"/>
       <c r="F20" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D23" s="9" t="s">
         <v>131</v>
       </c>
@@ -1772,7 +1784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D24" s="9" t="s">
         <v>131</v>
       </c>
@@ -1783,7 +1795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D25" s="9" t="s">
         <v>131</v>
       </c>
@@ -1794,9 +1806,35 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>